<commit_message>
Finished all 6 Questions
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vm35884\Documents\DA15\Excel\lookups-exercise-sunitha-m25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAADF69C-3B60-4ED2-8964-FED3A1D10B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B08ADE-0EF5-4712-92E1-6E558F847430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1178,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1265,7 +1265,7 @@
         <v>-4.3170750765267295E-2</v>
       </c>
       <c r="F2">
-        <f>IFERROR(RANK(E2,E2:E52,1),"-")</f>
+        <f>IFERROR(RANK(E2,$E$2:$E$52,1),"-")</f>
         <v>14</v>
       </c>
       <c r="G2">
@@ -1283,7 +1283,7 @@
         <v>-9.4972027086493035E-2</v>
       </c>
       <c r="K2">
-        <f>IFERROR(RANK(J2,J2:J52,1),"-")</f>
+        <f>IFERROR(RANK(J2,$J$2:$J$52,1),"-")</f>
         <v>10</v>
       </c>
       <c r="L2">
@@ -1301,7 +1301,7 @@
         <v>-5.6484362894991494E-2</v>
       </c>
       <c r="P2">
-        <f>IFERROR(RANK(O2,O2:O52,1),"-")</f>
+        <f>IFERROR(RANK(O2,$O$2:$O$52,1),"-")</f>
         <v>14</v>
       </c>
     </row>
@@ -1324,8 +1324,8 @@
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F52" si="2">IFERROR(RANK(E3,E3:E53,1),"-")</f>
-        <v>21</v>
+        <f t="shared" ref="F3:F52" si="2">IFERROR(RANK(E3,$E$2:$E$52,1),"-")</f>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>334800</v>
@@ -1342,8 +1342,8 @@
         <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">IFERROR(RANK(J3,J3:J53,1),"-")</f>
-        <v>13</v>
+        <f t="shared" ref="K3:K52" si="5">IFERROR(RANK(J3,$J$2:$J$52,1),"-")</f>
+        <v>14</v>
       </c>
       <c r="L3">
         <v>322700</v>
@@ -1360,8 +1360,8 @@
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="8">IFERROR(RANK(O3,O3:O53,1),"-")</f>
-        <v>36</v>
+        <f t="shared" ref="P3:P52" si="8">IFERROR(RANK(O3,$O$2:$O$52,1),"-")</f>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G4">
         <v>3652300</v>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L4">
         <v>3662400</v>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="P4">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1479,7 +1479,7 @@
       </c>
       <c r="P5">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="5"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="L6">
         <v>445200</v>
@@ -1538,7 +1538,7 @@
       </c>
       <c r="P6">
         <f t="shared" si="8"/>
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L7">
         <v>3345200</v>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L9">
         <v>10790500</v>
@@ -1715,7 +1715,7 @@
       </c>
       <c r="P9">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L10">
         <v>487500</v>
@@ -1774,7 +1774,7 @@
       </c>
       <c r="P10">
         <f t="shared" si="8"/>
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L12">
         <v>4677800</v>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="P12">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -1933,7 +1933,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="L13">
         <v>6207300</v>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="P13">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -1992,7 +1992,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="L14">
         <v>526200</v>
@@ -2010,7 +2010,7 @@
       </c>
       <c r="P14">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2033,7 +2033,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="G15">
         <v>184167800</v>
@@ -2051,7 +2051,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="L15">
         <v>188953500</v>
@@ -2069,7 +2069,7 @@
       </c>
       <c r="P15">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2092,7 +2092,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="L16">
         <v>7397200</v>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="P16">
         <f t="shared" si="8"/>
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2151,7 +2151,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="L17">
         <v>15311800</v>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="P17">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -2228,7 +2228,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="L18">
         <v>2910600</v>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="P18">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2269,7 +2269,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="L19">
         <v>9343000</v>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="P19">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2328,7 +2328,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="L20">
         <v>130621400</v>
@@ -2364,7 +2364,7 @@
       </c>
       <c r="P20">
         <f t="shared" si="8"/>
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2387,7 +2387,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -2405,7 +2405,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="L21">
         <v>24323000</v>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="P21">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="L22">
         <v>11935200</v>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="P22">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -2523,7 +2523,7 @@
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="L23">
         <v>23220300</v>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="P23">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -2582,7 +2582,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="L24">
         <v>1112600</v>
@@ -2600,7 +2600,7 @@
       </c>
       <c r="P24">
         <f t="shared" si="8"/>
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2623,7 +2623,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="L25">
         <v>496500</v>
@@ -2659,7 +2659,7 @@
       </c>
       <c r="P25">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -2700,7 +2700,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="L26">
         <v>5430700</v>
@@ -2718,7 +2718,7 @@
       </c>
       <c r="P26">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2800,7 +2800,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="P28">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2859,7 +2859,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="L29">
         <v>2889900</v>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="P29">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2918,7 +2918,7 @@
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -2936,7 +2936,7 @@
       </c>
       <c r="K30">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="L30">
         <v>12861300</v>
@@ -2954,7 +2954,7 @@
       </c>
       <c r="P30">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -2995,7 +2995,7 @@
       </c>
       <c r="K31">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="L31">
         <v>1870700</v>
@@ -3013,7 +3013,7 @@
       </c>
       <c r="P31">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3036,7 +3036,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -3054,7 +3054,7 @@
       </c>
       <c r="K32">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="L32">
         <v>6157400</v>
@@ -3072,7 +3072,7 @@
       </c>
       <c r="P32">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3095,7 +3095,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="K33">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="L33">
         <v>989572899.99999905</v>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="P33">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3154,7 +3154,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="G34">
         <v>4350600</v>
@@ -3172,7 +3172,7 @@
       </c>
       <c r="K34">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="L34">
         <v>4345600</v>
@@ -3190,7 +3190,7 @@
       </c>
       <c r="P34">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3272,7 +3272,7 @@
       </c>
       <c r="F36">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -3308,7 +3308,7 @@
       </c>
       <c r="P36">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="K37">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="L37">
         <v>2296900</v>
@@ -3367,7 +3367,7 @@
       </c>
       <c r="P37">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3390,7 +3390,7 @@
       </c>
       <c r="F38">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="K38">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="L38">
         <v>777800</v>
@@ -3426,7 +3426,7 @@
       </c>
       <c r="P38">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3449,7 +3449,7 @@
       </c>
       <c r="F39">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -3467,7 +3467,7 @@
       </c>
       <c r="K39">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L39">
         <v>1759500</v>
@@ -3485,7 +3485,7 @@
       </c>
       <c r="P39">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="F40">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="K40">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="L40">
         <v>40216700</v>
@@ -3544,7 +3544,7 @@
       </c>
       <c r="P40">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3567,7 +3567,7 @@
       </c>
       <c r="F41">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="K41">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="L41">
         <v>4799900</v>
@@ -3603,7 +3603,7 @@
       </c>
       <c r="P41">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3626,7 +3626,7 @@
       </c>
       <c r="F42">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -3644,7 +3644,7 @@
       </c>
       <c r="K42">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="L42">
         <v>199954600</v>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="P42">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3685,7 +3685,7 @@
       </c>
       <c r="F43">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -3703,7 +3703,7 @@
       </c>
       <c r="K43">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="L43">
         <v>8497500</v>
@@ -3721,7 +3721,7 @@
       </c>
       <c r="P43">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3744,7 +3744,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -3762,7 +3762,7 @@
       </c>
       <c r="K44">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="L44">
         <v>31282200</v>
@@ -3780,7 +3780,7 @@
       </c>
       <c r="P44">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3803,7 +3803,7 @@
       </c>
       <c r="F45">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="K45">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="L45">
         <v>56027100</v>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="P45">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="F46">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -3880,7 +3880,7 @@
       </c>
       <c r="K46">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="L46">
         <v>267100</v>
@@ -3898,7 +3898,7 @@
       </c>
       <c r="P46">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3921,7 +3921,7 @@
       </c>
       <c r="F47">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -3939,7 +3939,7 @@
       </c>
       <c r="K47">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="L47">
         <v>75072800</v>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="P47">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3980,7 +3980,7 @@
       </c>
       <c r="F48">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -3998,7 +3998,7 @@
       </c>
       <c r="K48">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="L48">
         <v>7289800</v>
@@ -4016,7 +4016,7 @@
       </c>
       <c r="P48">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="F49">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="K49">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -4098,7 +4098,7 @@
       </c>
       <c r="F50">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -4116,7 +4116,7 @@
       </c>
       <c r="K50">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="L50">
         <v>843200</v>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="P50">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4157,7 +4157,7 @@
       </c>
       <c r="F51">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -4175,7 +4175,7 @@
       </c>
       <c r="K51">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="L51">
         <v>8833900</v>
@@ -4193,7 +4193,7 @@
       </c>
       <c r="P51">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4216,7 +4216,7 @@
       </c>
       <c r="F52">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -4234,7 +4234,7 @@
       </c>
       <c r="K52">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L52">
         <v>2321600</v>
@@ -4252,7 +4252,7 @@
       </c>
       <c r="P52">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.55000000000000004">

</xml_diff>